<commit_message>
Add LiPo battery pack to BOM
Signed-off-by: Cristian Prundeanu <cristian.prundeanu@arm.com>
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for mbed-enablement-platform_F/BOM_mbed-enablement-platform_F.xlsx
+++ b/PCB/Project Outputs for mbed-enablement-platform_F/BOM_mbed-enablement-platform_F.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bencoo01\OneDrive - Arm\Documents\proj\pcb\fota-hardware\CLEANUP_PCB\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cripru01/work/ref-wem-hardware/PCB/Project Outputs for mbed-enablement-platform_F/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63D18D7-1B14-F442-A390-CC7E8F0B8E66}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7070"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30480" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="331">
   <si>
     <t>Qty</t>
   </si>
@@ -1002,13 +1003,31 @@
   </si>
   <si>
     <t>611-OS102011MA1QN1</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>3.7V 4400mAh</t>
+  </si>
+  <si>
+    <t>Lithium-Ion Battery Pack with protection circuit</t>
+  </si>
+  <si>
+    <t>485-354</t>
+  </si>
+  <si>
+    <t>1528-1834-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1028,6 +1047,12 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -1094,7 +1119,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1106,6 +1131,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2299,14 +2325,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.33203125" style="1" customWidth="1"/>
@@ -2321,7 +2345,7 @@
     <col min="12" max="256" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2391,7 +2415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>9</v>
       </c>
@@ -2426,7 +2450,7 @@
         <v>1458902</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>11</v>
       </c>
@@ -2461,7 +2485,7 @@
         <v>1327679</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -2496,7 +2520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2531,7 +2555,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2566,7 +2590,7 @@
         <v>1327666</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2599,7 +2623,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -2634,7 +2658,7 @@
         <v>1568026</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -2669,7 +2693,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -2704,7 +2728,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -2737,7 +2761,7 @@
       </c>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -2772,7 +2796,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -2807,7 +2831,7 @@
         <v>2322071</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -2842,7 +2866,7 @@
         <v>2322069</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -2877,7 +2901,7 @@
         <v>2322070</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2912,7 +2936,7 @@
         <v>1814269</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2947,7 +2971,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -2982,7 +3006,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -3017,7 +3041,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -3052,7 +3076,7 @@
         <v>2141071</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -3085,7 +3109,7 @@
       </c>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -3120,7 +3144,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>1</v>
       </c>
@@ -3155,7 +3179,7 @@
         <v>2059185</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>3</v>
       </c>
@@ -3190,7 +3214,7 @@
         <v>1652738</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>1</v>
       </c>
@@ -3225,7 +3249,7 @@
         <v>1469688</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>1</v>
       </c>
@@ -3260,7 +3284,7 @@
         <v>2302885</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -3295,7 +3319,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>1</v>
       </c>
@@ -3330,7 +3354,7 @@
         <v>1738856</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -3365,7 +3389,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>3</v>
       </c>
@@ -3400,7 +3424,7 @@
         <v>2302656</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>1</v>
       </c>
@@ -3433,7 +3457,7 @@
       </c>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>1</v>
       </c>
@@ -3466,7 +3490,7 @@
       </c>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>1</v>
       </c>
@@ -3499,7 +3523,7 @@
       </c>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>1</v>
       </c>
@@ -3534,7 +3558,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>1</v>
       </c>
@@ -3565,7 +3589,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>1</v>
       </c>
@@ -3600,7 +3624,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>1</v>
       </c>
@@ -3635,7 +3659,7 @@
         <v>2759860</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>1</v>
       </c>
@@ -3670,7 +3694,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>1</v>
       </c>
@@ -3705,7 +3729,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>1</v>
       </c>
@@ -3740,7 +3764,7 @@
         <v>1642489</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>1</v>
       </c>
@@ -3771,7 +3795,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1</v>
       </c>
@@ -3806,7 +3830,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1</v>
       </c>
@@ -3841,7 +3865,7 @@
         <v>2115658</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>1</v>
       </c>
@@ -3876,7 +3900,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>3</v>
       </c>
@@ -3911,7 +3935,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1</v>
       </c>
@@ -3946,7 +3970,7 @@
         <v>2474218</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -3981,9 +4005,36 @@
         <v>96</v>
       </c>
     </row>
+    <row r="49" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="K49" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:K48">
-    <sortCondition ref="E2:E48"/>
+  <sortState ref="A2:K49">
+    <sortCondition ref="E2:E49"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>